<commit_message>
code change after workspace change
</commit_message>
<xml_diff>
--- a/Vybex/src/test/resources/loginData.xlsx
+++ b/Vybex/src/test/resources/loginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rashid Mahmood\eclipse-workspace\BioYap\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Rashid SQA\Vybex\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254D51E6-F2E8-42C2-8C65-2157F65C9624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD84ACC-5EBF-4DE9-BCA9-428040394A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6EC91FE0-F11C-4870-BA6A-31E0F921FEF9}"/>
   </bookViews>
@@ -59,10 +59,10 @@
     <t>alison@yopmail.com</t>
   </si>
   <si>
-    <t>Test123</t>
-  </si>
-  <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +477,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -496,7 +496,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>

</xml_diff>